<commit_message>
Cập nhật Trạm quy hoạch bằng exels thì không cần phải nhập hết tất cả các trường thông tin... chỉ nhập trường key và trường thông tin muốn cập nhật
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/excel-templates/update_qh_netx_result.xlsx
+++ b/src/main/webapp/WEB-INF/excel-templates/update_qh_netx_result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Media_Soft\SVN_CTY\trunk\code\RIMS\src\main\webapp\WEB-INF\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\RIMS\source\RIMS\src\main\webapp\WEB-INF\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6CBF4B1C-AC2E-4826-B0DE-1C576DF05286}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{09FE6EA9-9975-4AAF-AEE9-1C6B1CC12AE1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="66">
   <si>
     <t>Thông tin chung</t>
   </si>
@@ -210,18 +210,6 @@
   </si>
   <si>
     <t>Kết quả</t>
-  </si>
-  <si>
-    <t>DEV_TEST2</t>
-  </si>
-  <si>
-    <t>18/01/2017</t>
-  </si>
-  <si>
-    <t>18/01/2018</t>
-  </si>
-  <si>
-    <t>BTC</t>
   </si>
   <si>
     <t>Kích cỡ (cao) (m)</t>
@@ -354,22 +342,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB4"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,319 +712,319 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB1" s="7"/>
+      <c r="N1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB1" s="9"/>
     </row>
     <row r="2" spans="1:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="5" t="s">
+      <c r="O2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AB2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AO2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="10" t="s">
+      <c r="AO2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="BB2" s="10" t="s">
+      <c r="BB2" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:54" s="3" customFormat="1" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1065,13 +1053,13 @@
         <v>29</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>30</v>
@@ -1104,13 +1092,13 @@
         <v>29</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AM3" s="2" t="s">
         <v>33</v>
@@ -1143,58 +1131,22 @@
         <v>29</v>
       </c>
       <c r="AW3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AX3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AY3" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AZ3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="BA3" s="11"/>
-      <c r="BB3" s="11"/>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
-      </c>
+      <c r="BA3" s="12"/>
+      <c r="BB3" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="M1:BB1"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
@@ -1207,6 +1159,16 @@
     <mergeCell ref="N2:Z2"/>
     <mergeCell ref="AA2:AM2"/>
     <mergeCell ref="AN2:AZ2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>